<commit_message>
Análisis y Diseño terminado
</commit_message>
<xml_diff>
--- a/cursos.xlsx
+++ b/cursos.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\esteb\OneDrive\Documentos\UNIVERSIDAD\POO\laboratorio_2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\esteb\Documents\UNIVERSITY\POO\laboratorio_2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0FA2697-FEA1-4DF8-BACD-5E60208F93EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14B07CB3-FC7C-42FB-A01E-649EBB4D0917}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4452" yWindow="348" windowWidth="17280" windowHeight="9960" xr2:uid="{DAD11EE4-B658-4D06-89B6-01533AEC2442}"/>
+    <workbookView xWindow="0" yWindow="4335" windowWidth="18000" windowHeight="9270" xr2:uid="{DAD11EE4-B658-4D06-89B6-01533AEC2442}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="26">
   <si>
     <t>id_sede</t>
   </si>
@@ -71,9 +71,6 @@
     <t>miercoles</t>
   </si>
   <si>
-    <t>cantiadad_estudiantes</t>
-  </si>
-  <si>
     <t>ciudadania</t>
   </si>
   <si>
@@ -102,6 +99,21 @@
   </si>
   <si>
     <t>viernes</t>
+  </si>
+  <si>
+    <t>cantidad_estudiantes</t>
+  </si>
+  <si>
+    <t>introduccion</t>
+  </si>
+  <si>
+    <t>sabado</t>
+  </si>
+  <si>
+    <t>algebra</t>
+  </si>
+  <si>
+    <t>quimica</t>
   </si>
 </sst>
 </file>
@@ -453,19 +465,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC24FDA2-8E1D-49BC-8415-42B9F18CE7A0}">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="22" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -485,10 +497,10 @@
         <v>5</v>
       </c>
       <c r="G1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -511,7 +523,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -534,7 +546,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -542,7 +554,7 @@
         <v>110</v>
       </c>
       <c r="C4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D4">
         <v>9</v>
@@ -557,7 +569,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -565,7 +577,7 @@
         <v>110</v>
       </c>
       <c r="C5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D5">
         <v>10</v>
@@ -580,7 +592,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -588,7 +600,7 @@
         <v>110</v>
       </c>
       <c r="C6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D6">
         <v>11</v>
@@ -603,7 +615,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -611,7 +623,7 @@
         <v>110</v>
       </c>
       <c r="C7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D7">
         <v>8</v>
@@ -620,13 +632,13 @@
         <v>2</v>
       </c>
       <c r="F7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G7">
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -634,7 +646,7 @@
         <v>110</v>
       </c>
       <c r="C8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D8">
         <v>9</v>
@@ -643,13 +655,13 @@
         <v>1</v>
       </c>
       <c r="F8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G8">
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -657,7 +669,7 @@
         <v>110</v>
       </c>
       <c r="C9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D9">
         <v>13</v>
@@ -672,7 +684,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -680,7 +692,7 @@
         <v>110</v>
       </c>
       <c r="C10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D10">
         <v>16</v>
@@ -689,13 +701,13 @@
         <v>2</v>
       </c>
       <c r="F10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G10">
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -703,7 +715,7 @@
         <v>110</v>
       </c>
       <c r="C11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D11">
         <v>14</v>
@@ -718,7 +730,77 @@
         <v>15</v>
       </c>
     </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>110</v>
+      </c>
+      <c r="C12" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12">
+        <v>12</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12" t="s">
+        <v>10</v>
+      </c>
+      <c r="G12">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>110</v>
+      </c>
+      <c r="C13" t="s">
+        <v>24</v>
+      </c>
+      <c r="D13">
+        <v>10</v>
+      </c>
+      <c r="E13">
+        <v>2</v>
+      </c>
+      <c r="F13" t="s">
+        <v>23</v>
+      </c>
+      <c r="G13">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>110</v>
+      </c>
+      <c r="C14" t="s">
+        <v>25</v>
+      </c>
+      <c r="D14">
+        <v>11</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="F14" t="s">
+        <v>20</v>
+      </c>
+      <c r="G14">
+        <v>23</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>